<commit_message>
DEV : ajout fonction lecture QUESU + fonction pour générer bons de commandes
</commit_message>
<xml_diff>
--- a/dev/fichier_exemple_commande/v2 prog EPTB2023_version dev libreSQE.xlsx
+++ b/dev/fichier_exemple_commande/v2 prog EPTB2023_version dev libreSQE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\LibreSQE\dev\fichier_exemple_commande\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6105C17-9E59-489E-AAC8-54EE79024C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28811AB2-E96D-4FD7-94CA-17AA597659CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionnaire_donnees" sheetId="9" r:id="rId1"/>
@@ -22,9 +22,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">calendrier!$A$1:$P$96</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">programme_annuel!$A$1:$G$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">programme_annuel!$A$1:$H$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">programmes_types!$A$1:$T$535</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">programme_annuel!$A$1:$G$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">programme_annuel!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8158" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8284" uniqueCount="1152">
   <si>
     <t>UG</t>
   </si>
@@ -3453,6 +3453,60 @@
   </si>
   <si>
     <t>sans objet</t>
+  </si>
+  <si>
+    <t>04376019</t>
+  </si>
+  <si>
+    <t>04376028</t>
+  </si>
+  <si>
+    <t>04376029</t>
+  </si>
+  <si>
+    <t>04376020</t>
+  </si>
+  <si>
+    <t>04376021</t>
+  </si>
+  <si>
+    <t>04376022</t>
+  </si>
+  <si>
+    <t>04390002</t>
+  </si>
+  <si>
+    <t>04373037</t>
+  </si>
+  <si>
+    <t>04373038</t>
+  </si>
+  <si>
+    <t>04373039</t>
+  </si>
+  <si>
+    <t>04373040</t>
+  </si>
+  <si>
+    <t>04373041</t>
+  </si>
+  <si>
+    <t>04376023</t>
+  </si>
+  <si>
+    <t>04376024</t>
+  </si>
+  <si>
+    <t>04376025</t>
+  </si>
+  <si>
+    <t>04376026</t>
+  </si>
+  <si>
+    <t>04376027</t>
+  </si>
+  <si>
+    <t>code_tmp</t>
   </si>
 </sst>
 </file>
@@ -3809,7 +3863,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="58">
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -4649,7 +4723,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5940,14 +6014,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G98" sqref="G98:G101"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5956,12 +6030,13 @@
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="23" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="57.5703125" customWidth="1"/>
-    <col min="6" max="6" width="125.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="57.5703125" customWidth="1"/>
+    <col min="7" max="7" width="125.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -5975,16 +6050,19 @@
         <v>447</v>
       </c>
       <c r="E1" s="10" t="s">
+        <v>1151</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>448</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>450</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>568</v>
       </c>
@@ -5994,20 +6072,23 @@
       <c r="C2" s="23" t="s">
         <v>574</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="23" t="s">
         <v>574</v>
       </c>
       <c r="E2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F2" t="s">
         <v>627</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>693</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -6017,20 +6098,23 @@
       <c r="C3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="23" t="s">
         <v>34</v>
       </c>
       <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" t="s">
         <v>628</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>694</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -6040,20 +6124,23 @@
       <c r="C4" s="23" t="s">
         <v>444</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="23" t="s">
         <v>444</v>
       </c>
       <c r="E4" t="s">
+        <v>444</v>
+      </c>
+      <c r="F4" t="s">
         <v>629</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>695</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -6063,20 +6150,23 @@
       <c r="C5" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="23" t="s">
         <v>142</v>
       </c>
       <c r="E5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F5" t="s">
         <v>143</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>695</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -6086,20 +6176,23 @@
       <c r="C6" s="23" t="s">
         <v>438</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="23" t="s">
         <v>438</v>
       </c>
       <c r="E6" t="s">
+        <v>438</v>
+      </c>
+      <c r="F6" t="s">
         <v>630</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>696</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -6109,20 +6202,23 @@
       <c r="C7" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="23" t="s">
         <v>140</v>
       </c>
       <c r="E7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F7" t="s">
         <v>141</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>695</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>41</v>
       </c>
@@ -6132,20 +6228,23 @@
       <c r="C8" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="23" t="s">
         <v>157</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
       <c r="F8" t="s">
+        <v>133</v>
+      </c>
+      <c r="G8" t="s">
         <v>695</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -6155,20 +6254,23 @@
       <c r="C9" s="23" t="s">
         <v>437</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="23" t="s">
         <v>437</v>
       </c>
       <c r="E9" t="s">
+        <v>437</v>
+      </c>
+      <c r="F9" t="s">
         <v>631</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>697</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -6178,20 +6280,23 @@
       <c r="C10" s="23" t="s">
         <v>443</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="23" t="s">
         <v>443</v>
       </c>
       <c r="E10" t="s">
+        <v>443</v>
+      </c>
+      <c r="F10" t="s">
         <v>632</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>698</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>568</v>
       </c>
@@ -6201,20 +6306,23 @@
       <c r="C11" s="23" t="s">
         <v>432</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="23" t="s">
         <v>432</v>
       </c>
       <c r="E11" t="s">
+        <v>432</v>
+      </c>
+      <c r="F11" t="s">
         <v>44</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>699</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>568</v>
       </c>
@@ -6224,20 +6332,23 @@
       <c r="C12" s="23" t="s">
         <v>575</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="23" t="s">
         <v>575</v>
       </c>
       <c r="E12" t="s">
+        <v>575</v>
+      </c>
+      <c r="F12" t="s">
         <v>633</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>693</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>568</v>
       </c>
@@ -6247,20 +6358,23 @@
       <c r="C13" s="23" t="s">
         <v>427</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="23" t="s">
         <v>427</v>
       </c>
       <c r="E13" t="s">
+        <v>427</v>
+      </c>
+      <c r="F13" t="s">
         <v>634</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>700</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>568</v>
       </c>
@@ -6270,20 +6384,23 @@
       <c r="C14" s="23" t="s">
         <v>428</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="23" t="s">
         <v>428</v>
       </c>
       <c r="E14" t="s">
+        <v>428</v>
+      </c>
+      <c r="F14" t="s">
         <v>635</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>700</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>568</v>
       </c>
@@ -6293,18 +6410,21 @@
       <c r="C15" s="23" t="s">
         <v>576</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="23" t="s">
         <v>576</v>
       </c>
       <c r="E15" t="s">
+        <v>576</v>
+      </c>
+      <c r="F15" t="s">
         <v>636</v>
       </c>
-      <c r="F15"/>
-      <c r="G15" t="s">
+      <c r="G15"/>
+      <c r="H15" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>568</v>
       </c>
@@ -6314,18 +6434,21 @@
       <c r="C16" s="23" t="s">
         <v>577</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="23" t="s">
         <v>577</v>
       </c>
       <c r="E16" t="s">
+        <v>577</v>
+      </c>
+      <c r="F16" t="s">
         <v>636</v>
       </c>
-      <c r="F16"/>
-      <c r="G16" t="s">
+      <c r="G16"/>
+      <c r="H16" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>568</v>
       </c>
@@ -6335,20 +6458,23 @@
       <c r="C17" s="23" t="s">
         <v>578</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="23" t="s">
         <v>578</v>
       </c>
       <c r="E17" t="s">
+        <v>578</v>
+      </c>
+      <c r="F17" t="s">
         <v>637</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>701</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>568</v>
       </c>
@@ -6358,20 +6484,23 @@
       <c r="C18" s="23" t="s">
         <v>430</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="23" t="s">
         <v>430</v>
       </c>
       <c r="E18" t="s">
+        <v>430</v>
+      </c>
+      <c r="F18" t="s">
         <v>43</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>702</v>
       </c>
-      <c r="G18" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>568</v>
       </c>
@@ -6381,20 +6510,23 @@
       <c r="C19" s="23" t="s">
         <v>429</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="23" t="s">
         <v>429</v>
       </c>
       <c r="E19" t="s">
+        <v>429</v>
+      </c>
+      <c r="F19" t="s">
         <v>42</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>703</v>
       </c>
-      <c r="G19" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>568</v>
       </c>
@@ -6404,20 +6536,23 @@
       <c r="C20" s="23" t="s">
         <v>431</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="23" t="s">
         <v>431</v>
       </c>
       <c r="E20" t="s">
+        <v>431</v>
+      </c>
+      <c r="F20" t="s">
         <v>638</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>704</v>
       </c>
-      <c r="G20" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>568</v>
       </c>
@@ -6427,20 +6562,23 @@
       <c r="C21" s="23" t="s">
         <v>579</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="23" t="s">
         <v>579</v>
       </c>
       <c r="E21" t="s">
+        <v>579</v>
+      </c>
+      <c r="F21" t="s">
         <v>639</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="G21" s="31" t="s">
         <v>705</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>568</v>
       </c>
@@ -6450,20 +6588,23 @@
       <c r="C22" s="23" t="s">
         <v>580</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="23" t="s">
         <v>580</v>
       </c>
       <c r="E22" t="s">
+        <v>580</v>
+      </c>
+      <c r="F22" t="s">
         <v>640</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>706</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>1127</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>568</v>
       </c>
@@ -6473,20 +6614,23 @@
       <c r="C23" s="23" t="s">
         <v>581</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="23" t="s">
         <v>581</v>
       </c>
       <c r="E23" t="s">
+        <v>581</v>
+      </c>
+      <c r="F23" t="s">
         <v>641</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>707</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -6496,20 +6640,23 @@
       <c r="C24" s="23" t="s">
         <v>426</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="23" t="s">
         <v>426</v>
       </c>
       <c r="E24" t="s">
+        <v>426</v>
+      </c>
+      <c r="F24" t="s">
         <v>642</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>708</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -6519,20 +6666,23 @@
       <c r="C25" s="23" t="s">
         <v>582</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="23" t="s">
         <v>582</v>
       </c>
       <c r="E25" t="s">
+        <v>582</v>
+      </c>
+      <c r="F25" t="s">
         <v>643</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>709</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -6542,20 +6692,23 @@
       <c r="C26" s="23" t="s">
         <v>583</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="23" t="s">
         <v>583</v>
       </c>
       <c r="E26" t="s">
+        <v>583</v>
+      </c>
+      <c r="F26" t="s">
         <v>644</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>710</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -6565,20 +6718,23 @@
       <c r="C27" s="23" t="s">
         <v>584</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="23" t="s">
         <v>584</v>
       </c>
       <c r="E27" t="s">
+        <v>584</v>
+      </c>
+      <c r="F27" t="s">
         <v>645</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>711</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>1126</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>568</v>
       </c>
@@ -6588,20 +6744,23 @@
       <c r="C28" s="23" t="s">
         <v>585</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="23" t="s">
         <v>585</v>
       </c>
       <c r="E28" t="s">
+        <v>585</v>
+      </c>
+      <c r="F28" t="s">
         <v>646</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>712</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -6611,20 +6770,23 @@
       <c r="C29" s="23" t="s">
         <v>586</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="23" t="s">
         <v>586</v>
       </c>
       <c r="E29" t="s">
+        <v>586</v>
+      </c>
+      <c r="F29" t="s">
         <v>647</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>713</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>41</v>
       </c>
@@ -6634,20 +6796,23 @@
       <c r="C30" s="23" t="s">
         <v>439</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="23" t="s">
         <v>439</v>
       </c>
       <c r="E30" t="s">
+        <v>439</v>
+      </c>
+      <c r="F30" t="s">
         <v>648</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>698</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>568</v>
       </c>
@@ -6657,20 +6822,23 @@
       <c r="C31" s="23" t="s">
         <v>587</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="23" t="s">
         <v>587</v>
       </c>
       <c r="E31" t="s">
+        <v>587</v>
+      </c>
+      <c r="F31" t="s">
         <v>649</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>714</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>572</v>
       </c>
@@ -6680,20 +6848,23 @@
       <c r="C32" s="23" t="s">
         <v>588</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="23" t="s">
         <v>588</v>
       </c>
       <c r="E32" t="s">
+        <v>588</v>
+      </c>
+      <c r="F32" t="s">
         <v>650</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>715</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>572</v>
       </c>
@@ -6703,20 +6874,23 @@
       <c r="C33" s="23" t="s">
         <v>589</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="23" t="s">
         <v>589</v>
       </c>
       <c r="E33" t="s">
+        <v>589</v>
+      </c>
+      <c r="F33" t="s">
         <v>651</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>716</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>572</v>
       </c>
@@ -6726,18 +6900,21 @@
       <c r="C34" s="23" t="s">
         <v>590</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="23" t="s">
         <v>590</v>
       </c>
       <c r="E34" t="s">
+        <v>590</v>
+      </c>
+      <c r="F34" t="s">
         <v>652</v>
       </c>
-      <c r="F34" s="27"/>
-      <c r="G34" t="s">
+      <c r="G34" s="27"/>
+      <c r="H34" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>572</v>
       </c>
@@ -6747,20 +6924,23 @@
       <c r="C35" s="23" t="s">
         <v>591</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="23" t="s">
         <v>591</v>
       </c>
       <c r="E35" t="s">
+        <v>591</v>
+      </c>
+      <c r="F35" t="s">
         <v>653</v>
       </c>
-      <c r="F35" s="27" t="s">
+      <c r="G35" s="27" t="s">
         <v>717</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>572</v>
       </c>
@@ -6770,20 +6950,23 @@
       <c r="C36" s="23" t="s">
         <v>592</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="23" t="s">
         <v>592</v>
       </c>
       <c r="E36" t="s">
+        <v>592</v>
+      </c>
+      <c r="F36" t="s">
         <v>654</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>718</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>1122</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>572</v>
       </c>
@@ -6793,18 +6976,21 @@
       <c r="C37" s="23" t="s">
         <v>593</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="23" t="s">
         <v>593</v>
       </c>
       <c r="E37" t="s">
+        <v>593</v>
+      </c>
+      <c r="F37" t="s">
         <v>655</v>
       </c>
-      <c r="F37" s="27"/>
-      <c r="G37" t="s">
+      <c r="G37" s="27"/>
+      <c r="H37" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
@@ -6814,20 +7000,23 @@
       <c r="C38" s="23" t="s">
         <v>440</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="23" t="s">
         <v>440</v>
       </c>
       <c r="E38" t="s">
+        <v>440</v>
+      </c>
+      <c r="F38" t="s">
         <v>656</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>719</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -6837,20 +7026,23 @@
       <c r="C39" s="23" t="s">
         <v>441</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="23" t="s">
         <v>441</v>
       </c>
       <c r="E39" t="s">
+        <v>441</v>
+      </c>
+      <c r="F39" t="s">
         <v>657</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>698</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -6860,20 +7052,23 @@
       <c r="C40" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="23" t="s">
         <v>158</v>
       </c>
       <c r="E40" t="s">
+        <v>158</v>
+      </c>
+      <c r="F40" t="s">
         <v>134</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>695</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -6883,20 +7078,23 @@
       <c r="C41" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="23" t="s">
         <v>159</v>
       </c>
       <c r="E41" t="s">
+        <v>159</v>
+      </c>
+      <c r="F41" t="s">
         <v>135</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>695</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -6906,20 +7104,23 @@
       <c r="C42" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="23" t="s">
         <v>160</v>
       </c>
       <c r="E42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F42" t="s">
         <v>136</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>695</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -6929,20 +7130,23 @@
       <c r="C43" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="23" t="s">
         <v>161</v>
       </c>
       <c r="E43" t="s">
+        <v>161</v>
+      </c>
+      <c r="F43" t="s">
         <v>137</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>695</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -6952,20 +7156,23 @@
       <c r="C44" s="23" t="s">
         <v>162</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="23" t="s">
         <v>162</v>
       </c>
       <c r="E44" t="s">
+        <v>162</v>
+      </c>
+      <c r="F44" t="s">
         <v>138</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>695</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -6975,20 +7182,23 @@
       <c r="C45" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="23" t="s">
         <v>163</v>
       </c>
       <c r="E45" t="s">
+        <v>163</v>
+      </c>
+      <c r="F45" t="s">
         <v>139</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>695</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -6998,20 +7208,23 @@
       <c r="C46" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="23" t="s">
         <v>35</v>
       </c>
       <c r="E46" t="s">
+        <v>35</v>
+      </c>
+      <c r="F46" t="s">
         <v>658</v>
       </c>
-      <c r="F46" t="s">
+      <c r="G46" t="s">
         <v>720</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -7021,20 +7234,23 @@
       <c r="C47" s="23" t="s">
         <v>446</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="23" t="s">
         <v>446</v>
       </c>
       <c r="E47" t="s">
+        <v>446</v>
+      </c>
+      <c r="F47" t="s">
         <v>36</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>720</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -7044,20 +7260,23 @@
       <c r="C48" s="23" t="s">
         <v>445</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="23" t="s">
         <v>445</v>
       </c>
       <c r="E48" t="s">
+        <v>445</v>
+      </c>
+      <c r="F48" t="s">
         <v>659</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>720</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -7067,20 +7286,23 @@
       <c r="C49" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="23" t="s">
         <v>145</v>
       </c>
       <c r="E49" t="s">
+        <v>145</v>
+      </c>
+      <c r="F49" t="s">
         <v>151</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>720</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>41</v>
       </c>
@@ -7090,20 +7312,23 @@
       <c r="C50" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="23" t="s">
         <v>144</v>
       </c>
       <c r="E50" t="s">
+        <v>144</v>
+      </c>
+      <c r="F50" t="s">
         <v>150</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>720</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>41</v>
       </c>
@@ -7113,20 +7338,23 @@
       <c r="C51" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="23" t="s">
         <v>149</v>
       </c>
       <c r="E51" t="s">
+        <v>149</v>
+      </c>
+      <c r="F51" t="s">
         <v>155</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>720</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>41</v>
       </c>
@@ -7136,20 +7364,23 @@
       <c r="C52" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="23" t="s">
         <v>148</v>
       </c>
       <c r="E52" t="s">
+        <v>148</v>
+      </c>
+      <c r="F52" t="s">
         <v>154</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>720</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>41</v>
       </c>
@@ -7159,20 +7390,23 @@
       <c r="C53" s="23" t="s">
         <v>147</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="23" t="s">
         <v>147</v>
       </c>
       <c r="E53" t="s">
+        <v>147</v>
+      </c>
+      <c r="F53" t="s">
         <v>153</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>720</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>41</v>
       </c>
@@ -7182,20 +7416,23 @@
       <c r="C54" s="23" t="s">
         <v>146</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="23" t="s">
         <v>146</v>
       </c>
       <c r="E54" t="s">
+        <v>146</v>
+      </c>
+      <c r="F54" t="s">
         <v>152</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>720</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>738</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>568</v>
       </c>
@@ -7205,20 +7442,23 @@
       <c r="C55" s="23" t="s">
         <v>594</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="23" t="s">
         <v>594</v>
       </c>
       <c r="E55" t="s">
+        <v>594</v>
+      </c>
+      <c r="F55" t="s">
         <v>660</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>714</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>568</v>
       </c>
@@ -7228,20 +7468,23 @@
       <c r="C56" s="23" t="s">
         <v>595</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="23" t="s">
         <v>595</v>
       </c>
       <c r="E56" t="s">
+        <v>595</v>
+      </c>
+      <c r="F56" t="s">
         <v>661</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>721</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>568</v>
       </c>
@@ -7251,20 +7494,23 @@
       <c r="C57" s="23" t="s">
         <v>596</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="23" t="s">
         <v>596</v>
       </c>
       <c r="E57" t="s">
+        <v>596</v>
+      </c>
+      <c r="F57" t="s">
         <v>662</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>722</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>568</v>
       </c>
@@ -7274,18 +7520,21 @@
       <c r="C58" s="23" t="s">
         <v>597</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="23" t="s">
         <v>597</v>
       </c>
       <c r="E58" t="s">
+        <v>597</v>
+      </c>
+      <c r="F58" t="s">
         <v>663</v>
       </c>
-      <c r="F58"/>
-      <c r="G58" t="s">
+      <c r="G58"/>
+      <c r="H58" t="s">
         <v>1125</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>41</v>
       </c>
@@ -7295,140 +7544,179 @@
       <c r="C59" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="23" t="s">
         <v>131</v>
       </c>
       <c r="E59" t="s">
+        <v>131</v>
+      </c>
+      <c r="F59" t="s">
         <v>664</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>723</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>41</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
       </c>
-      <c r="D60" t="s">
+      <c r="C60" s="23" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E60" t="s">
         <v>598</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>665</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>724</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>41</v>
       </c>
       <c r="B61" t="s">
         <v>41</v>
       </c>
-      <c r="D61" t="s">
+      <c r="C61" s="23" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D61" s="23" t="s">
+        <v>1135</v>
+      </c>
+      <c r="E61" t="s">
         <v>599</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>666</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>725</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>743</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>41</v>
       </c>
       <c r="B62" t="s">
         <v>41</v>
       </c>
-      <c r="D62" t="s">
+      <c r="C62" s="23" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D62" s="23" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E62" t="s">
         <v>600</v>
       </c>
-      <c r="E62" t="s">
+      <c r="F62" t="s">
         <v>666</v>
       </c>
-      <c r="F62" t="s">
+      <c r="G62" t="s">
         <v>726</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>41</v>
       </c>
       <c r="B63" t="s">
         <v>41</v>
       </c>
-      <c r="D63" t="s">
+      <c r="C63" s="23" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D63" s="23" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E63" t="s">
         <v>601</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>665</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>727</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>1118</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>41</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C64" s="23" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D64" s="23" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E64" t="s">
         <v>602</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>667</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>728</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>41</v>
       </c>
       <c r="B65" t="s">
         <v>41</v>
       </c>
-      <c r="D65" t="s">
+      <c r="C65" s="23" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D65" s="23" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E65" t="s">
         <v>603</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>668</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>724</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>568</v>
       </c>
@@ -7438,20 +7726,23 @@
       <c r="C66" s="23" t="s">
         <v>434</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="23" t="s">
         <v>434</v>
       </c>
       <c r="E66" t="s">
+        <v>434</v>
+      </c>
+      <c r="F66" t="s">
         <v>669</v>
       </c>
-      <c r="F66" t="s">
+      <c r="G66" t="s">
         <v>729</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>572</v>
       </c>
@@ -7461,18 +7752,21 @@
       <c r="C67" s="23" t="s">
         <v>604</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="23" t="s">
         <v>604</v>
       </c>
       <c r="E67" t="s">
+        <v>604</v>
+      </c>
+      <c r="F67" t="s">
         <v>670</v>
       </c>
-      <c r="F67" s="27"/>
-      <c r="G67" t="s">
+      <c r="G67" s="27"/>
+      <c r="H67" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>572</v>
       </c>
@@ -7482,18 +7776,21 @@
       <c r="C68" s="23" t="s">
         <v>605</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="23" t="s">
         <v>605</v>
       </c>
       <c r="E68" t="s">
+        <v>605</v>
+      </c>
+      <c r="F68" t="s">
         <v>671</v>
       </c>
-      <c r="F68" s="27"/>
-      <c r="G68" t="s">
+      <c r="G68" s="27"/>
+      <c r="H68" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>572</v>
       </c>
@@ -7503,18 +7800,21 @@
       <c r="C69" s="23" t="s">
         <v>606</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="23" t="s">
         <v>606</v>
       </c>
       <c r="E69" t="s">
+        <v>606</v>
+      </c>
+      <c r="F69" t="s">
         <v>672</v>
       </c>
-      <c r="F69" s="27"/>
-      <c r="G69" t="s">
+      <c r="G69" s="27"/>
+      <c r="H69" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>572</v>
       </c>
@@ -7524,18 +7824,21 @@
       <c r="C70" s="23" t="s">
         <v>607</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D70" s="23" t="s">
         <v>607</v>
       </c>
       <c r="E70" t="s">
+        <v>607</v>
+      </c>
+      <c r="F70" t="s">
         <v>673</v>
       </c>
-      <c r="F70" s="27"/>
-      <c r="G70" t="s">
+      <c r="G70" s="27"/>
+      <c r="H70" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>572</v>
       </c>
@@ -7545,18 +7848,21 @@
       <c r="C71" s="23" t="s">
         <v>608</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D71" s="23" t="s">
         <v>608</v>
       </c>
       <c r="E71" t="s">
+        <v>608</v>
+      </c>
+      <c r="F71" t="s">
         <v>674</v>
       </c>
-      <c r="F71" s="27"/>
-      <c r="G71" t="s">
+      <c r="G71" s="27"/>
+      <c r="H71" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>572</v>
       </c>
@@ -7566,18 +7872,21 @@
       <c r="C72" s="23" t="s">
         <v>609</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D72" s="23" t="s">
         <v>609</v>
       </c>
       <c r="E72" t="s">
+        <v>609</v>
+      </c>
+      <c r="F72" t="s">
         <v>675</v>
       </c>
-      <c r="F72"/>
-      <c r="G72" t="s">
+      <c r="G72"/>
+      <c r="H72" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>572</v>
       </c>
@@ -7587,18 +7896,21 @@
       <c r="C73" s="23" t="s">
         <v>610</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D73" s="23" t="s">
         <v>610</v>
       </c>
       <c r="E73" t="s">
+        <v>610</v>
+      </c>
+      <c r="F73" t="s">
         <v>676</v>
       </c>
-      <c r="F73"/>
-      <c r="G73" t="s">
+      <c r="G73"/>
+      <c r="H73" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>572</v>
       </c>
@@ -7608,18 +7920,21 @@
       <c r="C74" s="23" t="s">
         <v>611</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D74" s="23" t="s">
         <v>611</v>
       </c>
       <c r="E74" t="s">
+        <v>611</v>
+      </c>
+      <c r="F74" t="s">
         <v>677</v>
       </c>
-      <c r="F74" s="27"/>
-      <c r="G74" t="s">
+      <c r="G74" s="27"/>
+      <c r="H74" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>572</v>
       </c>
@@ -7629,18 +7944,21 @@
       <c r="C75" s="23" t="s">
         <v>612</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D75" s="23" t="s">
         <v>612</v>
       </c>
       <c r="E75" t="s">
+        <v>612</v>
+      </c>
+      <c r="F75" t="s">
         <v>678</v>
       </c>
-      <c r="F75" s="27"/>
-      <c r="G75" t="s">
+      <c r="G75" s="27"/>
+      <c r="H75" t="s">
         <v>1120</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>572</v>
       </c>
@@ -7650,128 +7968,167 @@
       <c r="C76" s="23" t="s">
         <v>613</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D76" s="23" t="s">
         <v>613</v>
       </c>
       <c r="E76" t="s">
+        <v>613</v>
+      </c>
+      <c r="F76" t="s">
         <v>679</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>730</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>572</v>
       </c>
       <c r="B77" t="s">
         <v>572</v>
       </c>
-      <c r="D77" t="s">
+      <c r="C77" s="23" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D77" s="23" t="s">
+        <v>1140</v>
+      </c>
+      <c r="E77" t="s">
         <v>614</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>680</v>
       </c>
-      <c r="F77"/>
-      <c r="G77" t="s">
+      <c r="G77"/>
+      <c r="H77" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>568</v>
       </c>
       <c r="B78" t="s">
         <v>573</v>
       </c>
-      <c r="D78" t="s">
+      <c r="C78" s="23" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D78" s="23" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E78" t="s">
         <v>615</v>
       </c>
-      <c r="E78" t="s">
+      <c r="F78" t="s">
         <v>681</v>
       </c>
-      <c r="F78"/>
-      <c r="G78" t="s">
+      <c r="G78"/>
+      <c r="H78" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>568</v>
       </c>
       <c r="B79" t="s">
         <v>573</v>
       </c>
-      <c r="D79" t="s">
+      <c r="C79" s="23" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D79" s="23" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E79" t="s">
         <v>616</v>
       </c>
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>681</v>
       </c>
-      <c r="F79"/>
-      <c r="G79" t="s">
+      <c r="G79"/>
+      <c r="H79" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>568</v>
       </c>
       <c r="B80" t="s">
         <v>573</v>
       </c>
-      <c r="D80" t="s">
+      <c r="C80" s="23" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D80" s="23" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E80" t="s">
         <v>617</v>
       </c>
-      <c r="E80" t="s">
+      <c r="F80" t="s">
         <v>682</v>
       </c>
-      <c r="F80"/>
-      <c r="G80" t="s">
+      <c r="G80"/>
+      <c r="H80" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>568</v>
       </c>
       <c r="B81" t="s">
         <v>573</v>
       </c>
-      <c r="D81" t="s">
+      <c r="C81" s="23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D81" s="23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="E81" t="s">
         <v>618</v>
       </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>683</v>
       </c>
-      <c r="F81"/>
-      <c r="G81" t="s">
+      <c r="G81"/>
+      <c r="H81" t="s">
         <v>740</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>568</v>
       </c>
       <c r="B82" t="s">
         <v>573</v>
       </c>
-      <c r="D82" t="s">
+      <c r="C82" s="23" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D82" s="23" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E82" t="s">
         <v>619</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>681</v>
       </c>
-      <c r="F82"/>
-      <c r="G82" t="s">
+      <c r="G82"/>
+      <c r="H82" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>568</v>
       </c>
@@ -7781,118 +8138,151 @@
       <c r="C83" s="23" t="s">
         <v>620</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D83" s="23" t="s">
         <v>620</v>
       </c>
       <c r="E83" t="s">
+        <v>620</v>
+      </c>
+      <c r="F83" t="s">
         <v>682</v>
       </c>
-      <c r="F83"/>
-      <c r="G83" t="s">
+      <c r="G83"/>
+      <c r="H83" t="s">
         <v>742</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>41</v>
       </c>
       <c r="B84" t="s">
         <v>41</v>
       </c>
-      <c r="D84" t="s">
+      <c r="C84" s="23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D84" s="23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E84" t="s">
         <v>621</v>
       </c>
-      <c r="E84" t="s">
+      <c r="F84" t="s">
         <v>668</v>
       </c>
-      <c r="F84" t="s">
+      <c r="G84" t="s">
         <v>727</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>1118</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>41</v>
       </c>
       <c r="B85" t="s">
         <v>41</v>
       </c>
-      <c r="D85" t="s">
+      <c r="C85" s="23" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D85" s="23" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E85" t="s">
         <v>622</v>
       </c>
-      <c r="E85" t="s">
+      <c r="F85" t="s">
         <v>684</v>
       </c>
-      <c r="F85" t="s">
+      <c r="G85" t="s">
         <v>727</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>1118</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>41</v>
       </c>
       <c r="B86" t="s">
         <v>41</v>
       </c>
-      <c r="D86" t="s">
+      <c r="C86" s="23" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D86" s="23" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E86" t="s">
         <v>623</v>
       </c>
-      <c r="E86" t="s">
+      <c r="F86" t="s">
         <v>685</v>
       </c>
-      <c r="F86" t="s">
+      <c r="G86" t="s">
         <v>727</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>1118</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>41</v>
       </c>
       <c r="B87" t="s">
         <v>41</v>
       </c>
-      <c r="D87" t="s">
+      <c r="C87" s="23" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D87" s="23" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E87" t="s">
         <v>624</v>
       </c>
-      <c r="E87" t="s">
+      <c r="F87" t="s">
         <v>686</v>
       </c>
-      <c r="F87" t="s">
+      <c r="G87" t="s">
         <v>731</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>41</v>
       </c>
       <c r="B88" t="s">
         <v>41</v>
       </c>
-      <c r="D88" t="s">
+      <c r="C88" s="23" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D88" s="23" t="s">
+        <v>1150</v>
+      </c>
+      <c r="E88" t="s">
         <v>625</v>
       </c>
-      <c r="E88" t="s">
+      <c r="F88" t="s">
         <v>687</v>
       </c>
-      <c r="F88" t="s">
+      <c r="G88" t="s">
         <v>732</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>1123</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>41</v>
       </c>
@@ -7902,20 +8292,23 @@
       <c r="C89" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D89" s="23" t="s">
         <v>35</v>
       </c>
       <c r="E89" t="s">
+        <v>35</v>
+      </c>
+      <c r="F89" t="s">
         <v>658</v>
       </c>
-      <c r="F89" t="s">
+      <c r="G89" t="s">
         <v>720</v>
       </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>41</v>
       </c>
@@ -7925,20 +8318,23 @@
       <c r="C90" s="23" t="s">
         <v>626</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D90" s="23" t="s">
         <v>626</v>
       </c>
       <c r="E90" t="s">
+        <v>626</v>
+      </c>
+      <c r="F90" t="s">
         <v>688</v>
       </c>
-      <c r="F90" t="s">
+      <c r="G90" t="s">
         <v>733</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>41</v>
       </c>
@@ -7948,20 +8344,23 @@
       <c r="C91" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D91" s="23" t="s">
         <v>442</v>
       </c>
       <c r="E91" t="s">
+        <v>442</v>
+      </c>
+      <c r="F91" t="s">
         <v>689</v>
       </c>
-      <c r="F91" t="s">
+      <c r="G91" t="s">
         <v>734</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>41</v>
       </c>
@@ -7971,20 +8370,23 @@
       <c r="C92" s="23" t="s">
         <v>425</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="23" t="s">
         <v>425</v>
       </c>
       <c r="E92" t="s">
+        <v>425</v>
+      </c>
+      <c r="F92" t="s">
         <v>690</v>
       </c>
-      <c r="F92" t="s">
+      <c r="G92" t="s">
         <v>698</v>
       </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>41</v>
       </c>
@@ -7994,20 +8396,23 @@
       <c r="C93" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D93" s="23" t="s">
         <v>39</v>
       </c>
       <c r="E93" t="s">
+        <v>39</v>
+      </c>
+      <c r="F93" t="s">
         <v>40</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="s">
         <v>735</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>41</v>
       </c>
@@ -8017,20 +8422,23 @@
       <c r="C94" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D94" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E94" t="s">
+        <v>37</v>
+      </c>
+      <c r="F94" t="s">
         <v>38</v>
       </c>
-      <c r="F94" t="s">
+      <c r="G94" t="s">
         <v>736</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>739</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>568</v>
       </c>
@@ -8040,20 +8448,23 @@
       <c r="C95" s="23" t="s">
         <v>435</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D95" s="23" t="s">
         <v>435</v>
       </c>
       <c r="E95" t="s">
+        <v>435</v>
+      </c>
+      <c r="F95" t="s">
         <v>691</v>
       </c>
-      <c r="F95" t="s">
+      <c r="G95" t="s">
         <v>737</v>
       </c>
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>568</v>
       </c>
@@ -8063,20 +8474,23 @@
       <c r="C96" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D96" s="23" t="s">
         <v>433</v>
       </c>
       <c r="E96" t="s">
+        <v>433</v>
+      </c>
+      <c r="F96" t="s">
         <v>45</v>
       </c>
-      <c r="F96" t="s">
+      <c r="G96" t="s">
         <v>729</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>568</v>
       </c>
@@ -8086,20 +8500,23 @@
       <c r="C97" s="23" t="s">
         <v>436</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D97" s="23" t="s">
         <v>436</v>
       </c>
       <c r="E97" t="s">
+        <v>436</v>
+      </c>
+      <c r="F97" t="s">
         <v>692</v>
       </c>
-      <c r="F97" t="s">
+      <c r="G97" t="s">
         <v>737</v>
       </c>
-      <c r="G97" t="s">
+      <c r="H97" t="s">
         <v>1121</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>568</v>
       </c>
@@ -8109,14 +8526,17 @@
       <c r="D98" t="s">
         <v>1128</v>
       </c>
-      <c r="F98" s="1" t="s">
+      <c r="E98" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G98" s="1" t="s">
         <v>1131</v>
       </c>
-      <c r="G98" s="58" t="s">
+      <c r="H98" s="58" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>572</v>
       </c>
@@ -8126,14 +8546,17 @@
       <c r="D99" t="s">
         <v>1128</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="E99" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G99" s="1" t="s">
         <v>1131</v>
       </c>
-      <c r="G99" s="58" t="s">
+      <c r="H99" s="58" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>41</v>
       </c>
@@ -8143,14 +8566,17 @@
       <c r="D100" t="s">
         <v>1128</v>
       </c>
-      <c r="F100" s="1" t="s">
+      <c r="E100" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G100" s="1" t="s">
         <v>1131</v>
       </c>
-      <c r="G100" s="58" t="s">
+      <c r="H100" s="58" t="s">
         <v>1129</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>568</v>
       </c>
@@ -8160,21 +8586,18 @@
       <c r="D101" t="s">
         <v>1128</v>
       </c>
-      <c r="F101" s="1" t="s">
+      <c r="E101" t="s">
+        <v>1128</v>
+      </c>
+      <c r="G101" s="1" t="s">
         <v>1132</v>
       </c>
-      <c r="G101" s="58" t="s">
+      <c r="H101" s="58" t="s">
         <v>1130</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G97" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="UGVE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="43" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
@@ -8182,10 +8605,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873A4119-B421-47B4-B521-95475D346CBB}">
-  <dimension ref="A1:P96"/>
+  <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="I101" sqref="I101"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12998,284 +13421,394 @@
         <v>1116</v>
       </c>
     </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" s="4">
+        <v>1</v>
+      </c>
+      <c r="D97" s="4">
+        <v>1</v>
+      </c>
+      <c r="E97" s="4">
+        <v>1</v>
+      </c>
+      <c r="F97" s="4">
+        <v>1</v>
+      </c>
+      <c r="G97" s="4">
+        <v>1</v>
+      </c>
+      <c r="H97" s="4">
+        <v>1</v>
+      </c>
+      <c r="I97" s="4">
+        <v>1</v>
+      </c>
+      <c r="J97" s="4">
+        <v>1</v>
+      </c>
+      <c r="K97" s="4">
+        <v>1</v>
+      </c>
+      <c r="L97" s="4">
+        <v>1</v>
+      </c>
+      <c r="M97" s="4">
+        <v>1</v>
+      </c>
+      <c r="N97" s="4">
+        <v>1</v>
+      </c>
+      <c r="O97" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="P97" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C98" s="4">
+        <v>1</v>
+      </c>
+      <c r="D98" s="4">
+        <v>1</v>
+      </c>
+      <c r="E98" s="4">
+        <v>1</v>
+      </c>
+      <c r="F98" s="4">
+        <v>1</v>
+      </c>
+      <c r="G98" s="4">
+        <v>1</v>
+      </c>
+      <c r="H98" s="4">
+        <v>1</v>
+      </c>
+      <c r="I98" s="4">
+        <v>1</v>
+      </c>
+      <c r="J98" s="4">
+        <v>1</v>
+      </c>
+      <c r="K98" s="4">
+        <v>1</v>
+      </c>
+      <c r="L98" s="4">
+        <v>1</v>
+      </c>
+      <c r="M98" s="4">
+        <v>1</v>
+      </c>
+      <c r="N98" s="4">
+        <v>1</v>
+      </c>
+      <c r="O98" s="4" t="s">
+        <v>744</v>
+      </c>
+      <c r="P98" t="s">
+        <v>1116</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:P96" xr:uid="{873A4119-B421-47B4-B521-95475D346CBB}"/>
   <conditionalFormatting sqref="C2:N32">
-    <cfRule type="cellIs" dxfId="55" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33:N33">
-    <cfRule type="cellIs" dxfId="54" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="62" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:N34">
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:N35">
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:N36">
-    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:N37">
-    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="58" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:N38">
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:N39">
-    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="56" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:N40">
-    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41:N41">
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42:N42">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:N43">
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="52" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:N44">
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:N45">
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="50" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:N46">
-    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47:N47">
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48:N48">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:N49">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="46" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50:N50">
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:N51">
-    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="44" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:N52">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53:N53">
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:N54">
-    <cfRule type="cellIs" dxfId="33" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:N55">
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="40" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56:N56">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57:N58">
-    <cfRule type="cellIs" dxfId="30" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59:N60">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:N61">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62:N62">
-    <cfRule type="cellIs" dxfId="27" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:N63">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="34" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64:N64">
-    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:N66">
-    <cfRule type="cellIs" dxfId="24" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67:N68">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:N69">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70:N70">
-    <cfRule type="cellIs" dxfId="21" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:N72">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C73:N74">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C75:N75">
-    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C76:N76">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77:N78">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C79:N80">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C81:N81">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C82:N82">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83:N84">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C85:N85">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86:N86">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="18" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87:N87">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C88:N88">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C89:N89">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90:N90">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="14" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:N91">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:N92">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C93:N93">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:N94">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95:N95">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C96:N96">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C97:N97">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C96:N96">
+  <conditionalFormatting sqref="C98:N98">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -13290,7 +13823,7 @@
   <dimension ref="A1:S535"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41611,7 +42144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC6AE468-9D97-4AF6-8A92-E91EECBFE118}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
conversion automatique unites dans verification fichiers
</commit_message>
<xml_diff>
--- a/dev/fichier_exemple_commande/v2 prog EPTB2023_version dev libreSQE.xlsx
+++ b/dev/fichier_exemple_commande/v2 prog EPTB2023_version dev libreSQE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\LibreSQE\dev\fichier_exemple_commande\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28811AB2-E96D-4FD7-94CA-17AA597659CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77629A4-C486-464B-9C9C-B73C8EBB5D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dictionnaire_donnees" sheetId="9" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8284" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8284" uniqueCount="1154">
   <si>
     <t>UG</t>
   </si>
@@ -3507,6 +3507,12 @@
   </si>
   <si>
     <t>code_tmp</t>
+  </si>
+  <si>
+    <t>fevrier</t>
+  </si>
+  <si>
+    <t>decembre</t>
   </si>
 </sst>
 </file>
@@ -6019,8 +6025,8 @@
   </sheetPr>
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
@@ -8607,14 +8613,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873A4119-B421-47B4-B521-95475D346CBB}">
   <dimension ref="A1:P98"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="E105" sqref="E105"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" customWidth="1"/>
@@ -8632,7 +8638,7 @@
         <v>422</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>423</v>
+        <v>1152</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>424</v>
@@ -8662,7 +8668,7 @@
         <v>420</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>421</v>
+        <v>1153</v>
       </c>
       <c r="O1" s="8" t="s">
         <v>165</v>
@@ -12721,7 +12727,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>740</v>
       </c>
@@ -12771,12 +12777,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>740</v>
       </c>
-      <c r="B84" s="21" t="s">
-        <v>539</v>
+      <c r="B84" s="53" t="s">
+        <v>535</v>
       </c>
       <c r="C84" s="4">
         <v>0</v>
@@ -12821,7 +12827,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>741</v>
       </c>
@@ -12871,12 +12877,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>741</v>
       </c>
-      <c r="B86" s="21" t="s">
-        <v>539</v>
+      <c r="B86" s="53" t="s">
+        <v>535</v>
       </c>
       <c r="C86" s="4">
         <v>0</v>
@@ -12921,7 +12927,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>742</v>
       </c>
@@ -12971,12 +12977,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>742</v>
       </c>
-      <c r="B88" s="21" t="s">
-        <v>539</v>
+      <c r="B88" s="53" t="s">
+        <v>535</v>
       </c>
       <c r="C88" s="4">
         <v>0</v>
@@ -13021,7 +13027,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>1125</v>
       </c>
@@ -13071,12 +13077,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>1125</v>
       </c>
-      <c r="B90" s="21" t="s">
-        <v>539</v>
+      <c r="B90" s="53" t="s">
+        <v>535</v>
       </c>
       <c r="C90" s="32">
         <v>0</v>
@@ -13121,7 +13127,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>1121</v>
       </c>
@@ -13171,12 +13177,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>1121</v>
       </c>
-      <c r="B92" s="21" t="s">
-        <v>539</v>
+      <c r="B92" s="53" t="s">
+        <v>535</v>
       </c>
       <c r="C92" s="32">
         <v>0</v>
@@ -13221,7 +13227,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>1127</v>
       </c>
@@ -13271,12 +13277,12 @@
         <v>412</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>1127</v>
       </c>
-      <c r="B94" s="21" t="s">
-        <v>539</v>
+      <c r="B94" s="53" t="s">
+        <v>535</v>
       </c>
       <c r="C94" s="32">
         <v>0</v>

</xml_diff>